<commit_message>
add new feeCal function.
</commit_message>
<xml_diff>
--- a/test/test-fee/test-data/A0001.xlsx
+++ b/test/test-fee/test-data/A0001.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joeylam/repo/njs/njstool/test/test-fee/test-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E80E1E09-E34C-B744-A731-46338E9E215E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD0EB8D0-F1D0-7D42-AC4D-9E06EB8BB67A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15760" xr2:uid="{78CF0ED5-08D6-F744-B285-E54D90BEA11B}"/>
   </bookViews>
@@ -71,7 +71,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -104,7 +104,7 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -427,7 +427,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="I2" sqref="I2:I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -494,6 +494,9 @@
       <c r="H2">
         <v>10000</v>
       </c>
+      <c r="I2" s="1">
+        <v>42856</v>
+      </c>
       <c r="J2">
         <v>10</v>
       </c>
@@ -523,6 +526,9 @@
       <c r="H3">
         <v>10000</v>
       </c>
+      <c r="I3" s="1">
+        <v>42887</v>
+      </c>
       <c r="J3">
         <v>11</v>
       </c>
@@ -552,6 +558,9 @@
       <c r="H4">
         <v>10000</v>
       </c>
+      <c r="I4" s="1">
+        <v>42917</v>
+      </c>
       <c r="J4">
         <v>12</v>
       </c>
@@ -581,6 +590,9 @@
       <c r="H5">
         <v>10000</v>
       </c>
+      <c r="I5" s="1">
+        <v>42948</v>
+      </c>
       <c r="J5">
         <v>11.5</v>
       </c>
@@ -610,6 +622,9 @@
       <c r="H6">
         <v>10000</v>
       </c>
+      <c r="I6" s="1">
+        <v>42979</v>
+      </c>
       <c r="J6">
         <v>11.7</v>
       </c>
@@ -638,6 +653,9 @@
       </c>
       <c r="H7">
         <v>10000</v>
+      </c>
+      <c r="I7" s="1">
+        <v>43009</v>
       </c>
       <c r="J7">
         <v>13</v>

</xml_diff>

<commit_message>
fix the syntax error
</commit_message>
<xml_diff>
--- a/test/test-fee/test-data/A0001.xlsx
+++ b/test/test-fee/test-data/A0001.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joeylam/repo/njs/njstool/test/test-fee/test-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD0EB8D0-F1D0-7D42-AC4D-9E06EB8BB67A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E6C3E2E-8FF8-7F45-A495-C06F48E7D317}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15760" xr2:uid="{78CF0ED5-08D6-F744-B285-E54D90BEA11B}"/>
   </bookViews>
@@ -27,36 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="13">
   <si>
-    <t>TXN_ID</t>
-  </si>
-  <si>
-    <t>ACCT_ID</t>
-  </si>
-  <si>
-    <t>TXN_SEQ</t>
-  </si>
-  <si>
-    <t>TXN_TYPE</t>
-  </si>
-  <si>
-    <t>TRADE_DATE</t>
-  </si>
-  <si>
-    <t>FUND_ID</t>
-  </si>
-  <si>
-    <t>VALN_DATE</t>
-  </si>
-  <si>
-    <t>TXN_UNIT</t>
-  </si>
-  <si>
-    <t>PROCESS_DATE</t>
-  </si>
-  <si>
-    <t>UNIT_COST</t>
-  </si>
-  <si>
     <t>A00001</t>
   </si>
   <si>
@@ -64,6 +34,36 @@
   </si>
   <si>
     <t>BUY</t>
+  </si>
+  <si>
+    <t>txnId</t>
+  </si>
+  <si>
+    <t>acctId</t>
+  </si>
+  <si>
+    <t>txnSeq</t>
+  </si>
+  <si>
+    <t>txnType</t>
+  </si>
+  <si>
+    <t>tradeDate</t>
+  </si>
+  <si>
+    <t>fundId</t>
+  </si>
+  <si>
+    <t>valnDate</t>
+  </si>
+  <si>
+    <t>unit</t>
+  </si>
+  <si>
+    <t>processDate</t>
+  </si>
+  <si>
+    <t>unitCost</t>
   </si>
 </sst>
 </file>
@@ -427,7 +427,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I7"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -439,34 +439,34 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="H1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="I1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="J1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -474,19 +474,19 @@
         <v>100001</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="E2" s="1">
         <v>42856</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="G2" s="1">
         <v>42856</v>
@@ -506,19 +506,19 @@
         <v>100002</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C3" s="2">
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="E3" s="1">
         <v>42887</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="G3" s="1">
         <v>42887</v>
@@ -538,19 +538,19 @@
         <v>100003</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C4" s="2">
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="E4" s="1">
         <v>42917</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="G4" s="1">
         <v>42917</v>
@@ -570,19 +570,19 @@
         <v>100004</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C5" s="2">
         <v>1</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="E5" s="1">
         <v>42948</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="G5" s="1">
         <v>42948</v>
@@ -602,19 +602,19 @@
         <v>100005</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C6" s="2">
         <v>1</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="E6" s="1">
         <v>42979</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="G6" s="1">
         <v>42979</v>
@@ -634,19 +634,19 @@
         <v>100006</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C7" s="2">
         <v>1</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="E7" s="1">
         <v>43009</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="G7" s="1">
         <v>43009</v>

</xml_diff>